<commit_message>
Update XFWB and XFZB mapping
Fix conversionfactor and uld slac mapping
</commit_message>
<xml_diff>
--- a/Documentation_website/docs/Orchestration/assets/Orchestration-1.2.0-XFWB-5.0.0-mapping.xlsx
+++ b/Documentation_website/docs/Orchestration/assets/Orchestration-1.2.0-XFWB-5.0.0-mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iataonline-my.sharepoint.com/personal/lambertc_iata_org/Documents/ONE Record/31 CXML mapping/Ochestration 1.2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{7A6CA4D8-11C1-4AD9-AA64-9849092C22BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84F009C5-CDA4-458C-ABEE-8832D404555A}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{7A6CA4D8-11C1-4AD9-AA64-9849092C22BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBD8D004-470F-4FEC-A62C-DFF41594BE69}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{FDB6F52B-EA41-4419-BE36-DF3522468846}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4522" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4524" uniqueCount="895">
   <si>
     <t>Date</t>
   </si>
@@ -2494,9 +2494,6 @@
     <t>ULD#tareWeight</t>
   </si>
   <si>
-    <t>ULD#slac</t>
-  </si>
-  <si>
     <t>ULD#uldTypeCode</t>
   </si>
   <si>
@@ -2724,6 +2721,15 @@
   </si>
   <si>
     <t>Use the Currency Unit of rateCharge as they are always expressed in Origin currency as per Resolution 600a</t>
+  </si>
+  <si>
+    <t>WaybillLineItem#conversionFactor</t>
+  </si>
+  <si>
+    <t>ULD#inUnitComposition</t>
+  </si>
+  <si>
+    <t>UnitComposition#slac</t>
   </si>
 </sst>
 </file>
@@ -12736,9 +12742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF50A8E-523E-4C20-8110-A0749E3DBA50}">
   <dimension ref="A1:W402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L272" sqref="L272"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N307" sqref="M307:N307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -12805,10 +12811,10 @@
       </c>
       <c r="K2" s="40"/>
       <c r="L2" s="38" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="M2" s="57" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="N2" s="58"/>
       <c r="O2" s="58"/>
@@ -12820,7 +12826,7 @@
       <c r="U2" s="58"/>
       <c r="V2" s="58"/>
       <c r="W2" s="7" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -12855,7 +12861,7 @@
       </c>
       <c r="K4" s="41"/>
       <c r="L4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="M4" s="28" t="s">
         <v>31</v>
@@ -13135,7 +13141,7 @@
       </c>
       <c r="K19" s="41"/>
       <c r="L19" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="M19" s="28" t="s">
         <v>31</v>
@@ -13447,7 +13453,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="41"/>
       <c r="L39" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="M39" s="28" t="s">
         <v>115</v>
@@ -13475,7 +13481,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="41"/>
       <c r="L40" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="M40" s="28" t="s">
         <v>115</v>
@@ -13505,7 +13511,7 @@
       </c>
       <c r="K41" s="41"/>
       <c r="L41" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="M41" s="28"/>
       <c r="W41" t="s">
@@ -13552,7 +13558,7 @@
       </c>
       <c r="K43" s="41"/>
       <c r="L43" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="M43" s="28"/>
       <c r="W43" t="s">
@@ -13599,7 +13605,7 @@
       </c>
       <c r="K45" s="41"/>
       <c r="L45" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="M45" s="28"/>
       <c r="W45" t="s">
@@ -13704,7 +13710,7 @@
       </c>
       <c r="K49" s="41"/>
       <c r="L49" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M49" s="28" t="s">
         <v>140</v>
@@ -13729,7 +13735,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="41"/>
       <c r="L50" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M50" s="28" t="s">
         <v>140</v>
@@ -13761,7 +13767,7 @@
         <v>182</v>
       </c>
       <c r="N51" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="O51" t="s">
         <v>169</v>
@@ -13786,7 +13792,7 @@
       <c r="J52" s="3"/>
       <c r="K52" s="41"/>
       <c r="L52" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="M52" s="28" t="s">
         <v>140</v>
@@ -13816,7 +13822,7 @@
       </c>
       <c r="K53" s="41"/>
       <c r="L53" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="M53" s="28" t="s">
         <v>140</v>
@@ -13845,7 +13851,7 @@
         <v>182</v>
       </c>
       <c r="N54" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="O54" t="s">
         <v>186</v>
@@ -13867,7 +13873,7 @@
       </c>
       <c r="K55" s="43"/>
       <c r="L55" s="46" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="M55" s="49" t="s">
         <v>140</v>
@@ -13904,7 +13910,7 @@
       <c r="J56" s="15"/>
       <c r="K56" s="43"/>
       <c r="L56" s="44" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="M56" s="49" t="s">
         <v>140</v>
@@ -13919,7 +13925,7 @@
         <v>198</v>
       </c>
       <c r="Q56" s="44" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="R56" s="44"/>
       <c r="S56" s="44"/>
@@ -13945,7 +13951,7 @@
       <c r="J57" s="15"/>
       <c r="K57" s="43"/>
       <c r="L57" s="44" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="M57" s="49" t="s">
         <v>140</v>
@@ -13960,7 +13966,7 @@
         <v>198</v>
       </c>
       <c r="Q57" s="44" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="R57" s="44"/>
       <c r="S57" s="44"/>
@@ -14023,7 +14029,7 @@
       <c r="J59" s="15"/>
       <c r="K59" s="43"/>
       <c r="L59" s="46" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="M59" s="49" t="s">
         <v>140</v>
@@ -14032,13 +14038,13 @@
         <v>191</v>
       </c>
       <c r="O59" s="44" t="s">
+        <v>865</v>
+      </c>
+      <c r="P59" s="44" t="s">
         <v>866</v>
       </c>
-      <c r="P59" s="44" t="s">
+      <c r="Q59" s="44" t="s">
         <v>867</v>
-      </c>
-      <c r="Q59" s="44" t="s">
-        <v>868</v>
       </c>
       <c r="R59" s="44"/>
       <c r="S59" s="44"/>
@@ -14188,7 +14194,7 @@
         <v>214</v>
       </c>
       <c r="R63" s="44" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="S63" s="44"/>
       <c r="T63" s="50"/>
@@ -14213,7 +14219,7 @@
       <c r="J64" s="15"/>
       <c r="K64" s="43"/>
       <c r="L64" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M64" s="49" t="s">
         <v>140</v>
@@ -14256,7 +14262,7 @@
       <c r="J65" s="15"/>
       <c r="K65" s="43"/>
       <c r="L65" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M65" s="49"/>
       <c r="N65" s="44"/>
@@ -14287,7 +14293,7 @@
       <c r="J66" s="15"/>
       <c r="K66" s="43"/>
       <c r="L66" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M66" s="49" t="s">
         <v>140</v>
@@ -14597,7 +14603,7 @@
       <c r="J75" s="15"/>
       <c r="K75" s="43"/>
       <c r="L75" s="52" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="M75" s="49" t="s">
         <v>140</v>
@@ -14670,7 +14676,7 @@
       <c r="J78" s="15"/>
       <c r="K78" s="43"/>
       <c r="L78" s="52" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="M78" s="49" t="s">
         <v>140</v>
@@ -14744,7 +14750,7 @@
       <c r="J81" s="15"/>
       <c r="K81" s="43"/>
       <c r="L81" s="52" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="M81" s="49" t="s">
         <v>140</v>
@@ -14818,7 +14824,7 @@
       <c r="J84" s="15"/>
       <c r="K84" s="43"/>
       <c r="L84" s="52" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="M84" s="49" t="s">
         <v>140</v>
@@ -14923,7 +14929,7 @@
       </c>
       <c r="K88" s="43"/>
       <c r="L88" s="46" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="M88" s="49" t="s">
         <v>140</v>
@@ -14960,7 +14966,7 @@
       <c r="J89" s="15"/>
       <c r="K89" s="43"/>
       <c r="L89" s="44" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="M89" s="49" t="s">
         <v>140</v>
@@ -14999,7 +15005,7 @@
       <c r="J90" s="15"/>
       <c r="K90" s="43"/>
       <c r="L90" s="44" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="M90" s="49" t="s">
         <v>140</v>
@@ -15075,7 +15081,7 @@
       <c r="J92" s="15"/>
       <c r="K92" s="43"/>
       <c r="L92" s="46" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="M92" s="49" t="s">
         <v>140</v>
@@ -15084,13 +15090,13 @@
         <v>191</v>
       </c>
       <c r="O92" s="44" t="s">
+        <v>865</v>
+      </c>
+      <c r="P92" s="44" t="s">
         <v>866</v>
       </c>
-      <c r="P92" s="44" t="s">
+      <c r="Q92" s="44" t="s">
         <v>867</v>
-      </c>
-      <c r="Q92" s="44" t="s">
-        <v>868</v>
       </c>
       <c r="R92" s="44"/>
       <c r="S92" s="44"/>
@@ -15240,7 +15246,7 @@
         <v>214</v>
       </c>
       <c r="R96" s="44" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="S96" s="44"/>
       <c r="T96" s="50"/>
@@ -15265,7 +15271,7 @@
       <c r="J97" s="15"/>
       <c r="K97" s="43"/>
       <c r="L97" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M97" s="49" t="s">
         <v>140</v>
@@ -15308,7 +15314,7 @@
       <c r="J98" s="15"/>
       <c r="K98" s="43"/>
       <c r="L98" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M98" s="49"/>
       <c r="N98" s="44"/>
@@ -15339,7 +15345,7 @@
       <c r="J99" s="15"/>
       <c r="K99" s="43"/>
       <c r="L99" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M99" s="49" t="s">
         <v>140</v>
@@ -15649,7 +15655,7 @@
       <c r="J108" s="15"/>
       <c r="K108" s="43"/>
       <c r="L108" s="52" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="M108" s="49" t="s">
         <v>140</v>
@@ -15722,7 +15728,7 @@
       <c r="J111" s="15"/>
       <c r="K111" s="43"/>
       <c r="L111" s="52" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="M111" s="49" t="s">
         <v>140</v>
@@ -15796,7 +15802,7 @@
       <c r="J114" s="15"/>
       <c r="K114" s="43"/>
       <c r="L114" s="52" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="M114" s="49" t="s">
         <v>140</v>
@@ -15870,7 +15876,7 @@
       <c r="J117" s="15"/>
       <c r="K117" s="43"/>
       <c r="L117" s="52" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="M117" s="49" t="s">
         <v>140</v>
@@ -15975,7 +15981,7 @@
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="46" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="M121" s="49" t="s">
         <v>140</v>
@@ -16012,7 +16018,7 @@
       <c r="J122" s="14"/>
       <c r="K122" s="43"/>
       <c r="L122" s="44" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="M122" s="49" t="s">
         <v>140</v>
@@ -16051,7 +16057,7 @@
       <c r="J123" s="14"/>
       <c r="K123" s="43"/>
       <c r="L123" s="44" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="M123" s="49" t="s">
         <v>140</v>
@@ -16127,7 +16133,7 @@
       <c r="J125" s="14"/>
       <c r="K125" s="43"/>
       <c r="L125" s="46" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="M125" s="49" t="s">
         <v>140</v>
@@ -16136,13 +16142,13 @@
         <v>191</v>
       </c>
       <c r="O125" s="44" t="s">
+        <v>865</v>
+      </c>
+      <c r="P125" s="44" t="s">
         <v>866</v>
       </c>
-      <c r="P125" s="44" t="s">
+      <c r="Q125" s="44" t="s">
         <v>867</v>
-      </c>
-      <c r="Q125" s="44" t="s">
-        <v>868</v>
       </c>
       <c r="R125" s="44"/>
       <c r="S125" s="44"/>
@@ -16329,7 +16335,7 @@
         <v>214</v>
       </c>
       <c r="R130" s="44" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="S130" s="44"/>
       <c r="T130" s="50"/>
@@ -16354,7 +16360,7 @@
       <c r="J131" s="14"/>
       <c r="K131" s="43"/>
       <c r="L131" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M131" s="49" t="s">
         <v>140</v>
@@ -16397,7 +16403,7 @@
       <c r="J132" s="14"/>
       <c r="K132" s="43"/>
       <c r="L132" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M132" s="49"/>
       <c r="N132" s="44"/>
@@ -16428,7 +16434,7 @@
       <c r="J133" s="14"/>
       <c r="K133" s="43"/>
       <c r="L133" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M133" s="49" t="s">
         <v>140</v>
@@ -16823,7 +16829,7 @@
       <c r="J145" s="14"/>
       <c r="K145" s="43"/>
       <c r="L145" s="52" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="M145" s="49" t="s">
         <v>140</v>
@@ -16902,7 +16908,7 @@
       <c r="J148" s="14"/>
       <c r="K148" s="43"/>
       <c r="L148" s="52" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="M148" s="49" t="s">
         <v>140</v>
@@ -16982,7 +16988,7 @@
       <c r="J151" s="14"/>
       <c r="K151" s="43"/>
       <c r="L151" s="52" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="M151" s="49" t="s">
         <v>140</v>
@@ -17062,7 +17068,7 @@
       <c r="J154" s="14"/>
       <c r="K154" s="43"/>
       <c r="L154" s="52" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="M154" s="49" t="s">
         <v>140</v>
@@ -17310,7 +17316,7 @@
       <c r="J162" s="13"/>
       <c r="K162" s="43"/>
       <c r="L162" s="44" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M162" s="49" t="s">
         <v>140</v>
@@ -17468,7 +17474,7 @@
         <v>214</v>
       </c>
       <c r="R167" s="44" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="S167" s="44"/>
       <c r="T167" s="50"/>
@@ -17491,7 +17497,7 @@
       <c r="J168" s="3"/>
       <c r="K168" s="43"/>
       <c r="L168" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M168" s="49" t="s">
         <v>140</v>
@@ -17532,7 +17538,7 @@
       <c r="J169" s="3"/>
       <c r="K169" s="43"/>
       <c r="L169" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M169" s="49"/>
       <c r="N169" s="44"/>
@@ -17561,7 +17567,7 @@
       <c r="J170" s="3"/>
       <c r="K170" s="43"/>
       <c r="L170" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M170" s="49" t="s">
         <v>140</v>
@@ -17969,7 +17975,7 @@
       <c r="J184" s="3"/>
       <c r="K184" s="43"/>
       <c r="L184" s="52" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="M184" s="49" t="s">
         <v>140</v>
@@ -18033,7 +18039,7 @@
       <c r="J187" s="3"/>
       <c r="K187" s="43"/>
       <c r="L187" s="52" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="M187" s="49" t="s">
         <v>140</v>
@@ -18099,7 +18105,7 @@
       <c r="J190" s="3"/>
       <c r="K190" s="43"/>
       <c r="L190" s="52" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="M190" s="49" t="s">
         <v>140</v>
@@ -18164,7 +18170,7 @@
       <c r="J193" s="3"/>
       <c r="K193" s="43"/>
       <c r="L193" s="52" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="M193" s="49" t="s">
         <v>140</v>
@@ -18398,16 +18404,16 @@
       <c r="J206" s="3"/>
       <c r="K206" s="41"/>
       <c r="L206" s="45" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="M206" s="28" t="s">
         <v>182</v>
       </c>
       <c r="N206" t="s">
+        <v>819</v>
+      </c>
+      <c r="O206" t="s">
         <v>820</v>
-      </c>
-      <c r="O206" t="s">
-        <v>821</v>
       </c>
       <c r="P206" t="s">
         <v>373</v>
@@ -18429,16 +18435,16 @@
       <c r="J207" s="3"/>
       <c r="K207" s="41"/>
       <c r="L207" s="45" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="M207" s="28" t="s">
         <v>182</v>
       </c>
       <c r="N207" t="s">
+        <v>819</v>
+      </c>
+      <c r="O207" t="s">
         <v>820</v>
-      </c>
-      <c r="O207" t="s">
-        <v>821</v>
       </c>
       <c r="P207" t="s">
         <v>377</v>
@@ -18486,10 +18492,10 @@
         <v>182</v>
       </c>
       <c r="N209" t="s">
+        <v>819</v>
+      </c>
+      <c r="O209" t="s">
         <v>820</v>
-      </c>
-      <c r="O209" t="s">
-        <v>821</v>
       </c>
       <c r="P209" t="s">
         <v>384</v>
@@ -18515,10 +18521,10 @@
         <v>182</v>
       </c>
       <c r="N210" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="O210" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="211" spans="3:19" x14ac:dyDescent="0.25">
@@ -18554,19 +18560,19 @@
       </c>
       <c r="K212" s="41"/>
       <c r="L212" s="46" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="M212" s="28" t="s">
         <v>182</v>
       </c>
       <c r="N212" t="s">
+        <v>819</v>
+      </c>
+      <c r="O212" t="s">
         <v>820</v>
       </c>
-      <c r="O212" t="s">
-        <v>821</v>
-      </c>
       <c r="P212" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="Q212" t="s">
         <v>192</v>
@@ -18601,16 +18607,16 @@
       <c r="J214" s="3"/>
       <c r="K214" s="41"/>
       <c r="L214" s="45" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="M214" s="28" t="s">
         <v>182</v>
       </c>
       <c r="N214" t="s">
+        <v>819</v>
+      </c>
+      <c r="O214" t="s">
         <v>820</v>
-      </c>
-      <c r="O214" t="s">
-        <v>821</v>
       </c>
       <c r="P214" t="s">
         <v>398</v>
@@ -18641,10 +18647,10 @@
         <v>182</v>
       </c>
       <c r="N215" t="s">
+        <v>819</v>
+      </c>
+      <c r="O215" t="s">
         <v>820</v>
-      </c>
-      <c r="O215" t="s">
-        <v>821</v>
       </c>
       <c r="P215" t="s">
         <v>398</v>
@@ -18693,10 +18699,10 @@
         <v>182</v>
       </c>
       <c r="N217" t="s">
+        <v>819</v>
+      </c>
+      <c r="O217" t="s">
         <v>820</v>
-      </c>
-      <c r="O217" t="s">
-        <v>821</v>
       </c>
       <c r="P217" t="s">
         <v>413</v>
@@ -18725,10 +18731,10 @@
         <v>182</v>
       </c>
       <c r="N218" t="s">
+        <v>819</v>
+      </c>
+      <c r="O218" t="s">
         <v>820</v>
-      </c>
-      <c r="O218" t="s">
-        <v>821</v>
       </c>
       <c r="P218" t="s">
         <v>413</v>
@@ -18757,10 +18763,10 @@
         <v>182</v>
       </c>
       <c r="N219" t="s">
+        <v>819</v>
+      </c>
+      <c r="O219" t="s">
         <v>820</v>
-      </c>
-      <c r="O219" t="s">
-        <v>821</v>
       </c>
       <c r="P219" t="s">
         <v>413</v>
@@ -18802,16 +18808,16 @@
       <c r="J222" s="3"/>
       <c r="K222" s="41"/>
       <c r="L222" s="45" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="M222" s="28" t="s">
         <v>182</v>
       </c>
       <c r="N222" t="s">
+        <v>819</v>
+      </c>
+      <c r="O222" t="s">
         <v>820</v>
-      </c>
-      <c r="O222" t="s">
-        <v>821</v>
       </c>
       <c r="P222" t="s">
         <v>398</v>
@@ -18842,10 +18848,10 @@
         <v>182</v>
       </c>
       <c r="N223" t="s">
+        <v>819</v>
+      </c>
+      <c r="O223" t="s">
         <v>820</v>
-      </c>
-      <c r="O223" t="s">
-        <v>821</v>
       </c>
       <c r="P223" t="s">
         <v>398</v>
@@ -18892,10 +18898,10 @@
         <v>182</v>
       </c>
       <c r="N225" t="s">
+        <v>819</v>
+      </c>
+      <c r="O225" t="s">
         <v>820</v>
-      </c>
-      <c r="O225" t="s">
-        <v>821</v>
       </c>
       <c r="P225" t="s">
         <v>429</v>
@@ -18924,10 +18930,10 @@
         <v>182</v>
       </c>
       <c r="N226" t="s">
+        <v>819</v>
+      </c>
+      <c r="O226" t="s">
         <v>820</v>
-      </c>
-      <c r="O226" t="s">
-        <v>821</v>
       </c>
       <c r="P226" t="s">
         <v>429</v>
@@ -18956,10 +18962,10 @@
         <v>182</v>
       </c>
       <c r="N227" t="s">
+        <v>819</v>
+      </c>
+      <c r="O227" t="s">
         <v>820</v>
-      </c>
-      <c r="O227" t="s">
-        <v>821</v>
       </c>
       <c r="P227" t="s">
         <v>429</v>
@@ -19033,10 +19039,10 @@
         <v>140</v>
       </c>
       <c r="N232" t="s">
+        <v>819</v>
+      </c>
+      <c r="O232" t="s">
         <v>820</v>
-      </c>
-      <c r="O232" t="s">
-        <v>821</v>
       </c>
       <c r="P232" t="s">
         <v>392</v>
@@ -19065,10 +19071,10 @@
         <v>140</v>
       </c>
       <c r="N233" t="s">
+        <v>819</v>
+      </c>
+      <c r="O233" t="s">
         <v>820</v>
-      </c>
-      <c r="O233" t="s">
-        <v>821</v>
       </c>
       <c r="P233" t="s">
         <v>392</v>
@@ -19097,10 +19103,10 @@
         <v>140</v>
       </c>
       <c r="N234" t="s">
+        <v>819</v>
+      </c>
+      <c r="O234" t="s">
         <v>820</v>
-      </c>
-      <c r="O234" t="s">
-        <v>821</v>
       </c>
       <c r="P234" t="s">
         <v>392</v>
@@ -19145,10 +19151,10 @@
         <v>140</v>
       </c>
       <c r="N236" t="s">
+        <v>819</v>
+      </c>
+      <c r="O236" t="s">
         <v>820</v>
-      </c>
-      <c r="O236" t="s">
-        <v>821</v>
       </c>
       <c r="P236" t="s">
         <v>451</v>
@@ -19291,7 +19297,7 @@
         <v>140</v>
       </c>
       <c r="N244" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="245" spans="2:23" x14ac:dyDescent="0.25">
@@ -19367,7 +19373,7 @@
         <v>140</v>
       </c>
       <c r="N248" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="W248" t="s">
         <v>472</v>
@@ -19502,7 +19508,7 @@
       <c r="J255" s="3"/>
       <c r="K255" s="42"/>
       <c r="L255" s="22" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="M255" s="28" t="s">
         <v>140</v>
@@ -19511,7 +19517,7 @@
         <v>485</v>
       </c>
       <c r="O255" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="256" spans="2:23" x14ac:dyDescent="0.25">
@@ -19620,7 +19626,7 @@
       </c>
       <c r="K259" s="41"/>
       <c r="L259" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M259" s="28" t="s">
         <v>140</v>
@@ -19838,16 +19844,16 @@
       </c>
       <c r="K271" s="42"/>
       <c r="L271" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="M271" s="28" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N271" t="s">
         <v>724</v>
       </c>
       <c r="O271" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="272" spans="2:15" x14ac:dyDescent="0.25">
@@ -20393,16 +20399,16 @@
       </c>
       <c r="K298" s="42"/>
       <c r="L298" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="M298" s="28" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="N298" t="s">
         <v>724</v>
       </c>
       <c r="O298" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="299" spans="2:23" x14ac:dyDescent="0.25">
@@ -20421,10 +20427,10 @@
       <c r="J299" s="3"/>
       <c r="K299" s="42"/>
       <c r="L299" t="s">
+        <v>854</v>
+      </c>
+      <c r="M299" s="28" t="s">
         <v>855</v>
-      </c>
-      <c r="M299" s="28" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="300" spans="2:23" x14ac:dyDescent="0.25">
@@ -20487,19 +20493,19 @@
         <v>614</v>
       </c>
       <c r="N302" t="s">
+        <v>825</v>
+      </c>
+      <c r="O302" t="s">
         <v>826</v>
       </c>
-      <c r="O302" t="s">
-        <v>827</v>
-      </c>
       <c r="P302" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="Q302" t="s">
         <v>810</v>
       </c>
       <c r="W302" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="303" spans="2:23" x14ac:dyDescent="0.25">
@@ -20520,13 +20526,13 @@
       </c>
       <c r="K303" s="41"/>
       <c r="L303" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M303" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N303" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="304" spans="2:23" x14ac:dyDescent="0.25">
@@ -20547,13 +20553,13 @@
       </c>
       <c r="K304" s="41"/>
       <c r="L304" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M304" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N304" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="305" spans="4:23" x14ac:dyDescent="0.25">
@@ -20578,7 +20584,7 @@
         <v>614</v>
       </c>
       <c r="N305" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="306" spans="4:23" x14ac:dyDescent="0.25">
@@ -20603,13 +20609,13 @@
         <v>614</v>
       </c>
       <c r="N306" t="s">
+        <v>825</v>
+      </c>
+      <c r="O306" t="s">
         <v>826</v>
       </c>
-      <c r="O306" t="s">
-        <v>827</v>
-      </c>
       <c r="W306" s="37" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="307" spans="4:23" x14ac:dyDescent="0.25">
@@ -20627,10 +20633,13 @@
       </c>
       <c r="J307" s="3"/>
       <c r="K307" s="42"/>
-      <c r="L307" t="s">
-        <v>529</v>
-      </c>
-      <c r="M307" s="28"/>
+      <c r="L307"/>
+      <c r="M307" s="28" t="s">
+        <v>614</v>
+      </c>
+      <c r="N307" t="s">
+        <v>892</v>
+      </c>
     </row>
     <row r="308" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D308" t="s">
@@ -20692,10 +20701,10 @@
         <v>614</v>
       </c>
       <c r="N310" t="s">
+        <v>825</v>
+      </c>
+      <c r="O310" t="s">
         <v>826</v>
-      </c>
-      <c r="O310" t="s">
-        <v>827</v>
       </c>
       <c r="P310" t="s">
         <v>812</v>
@@ -20745,16 +20754,16 @@
       </c>
       <c r="K313" s="41"/>
       <c r="L313" s="52" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M313" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N313" t="s">
+        <v>825</v>
+      </c>
+      <c r="O313" t="s">
         <v>826</v>
-      </c>
-      <c r="O313" t="s">
-        <v>827</v>
       </c>
       <c r="P313" t="s">
         <v>813</v>
@@ -20810,7 +20819,7 @@
         <v>614</v>
       </c>
       <c r="N316" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O316" t="s">
         <v>814</v>
@@ -20832,13 +20841,13 @@
       <c r="J317" s="3"/>
       <c r="K317" s="41"/>
       <c r="L317" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M317" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N317" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O317" t="s">
         <v>815</v>
@@ -20864,10 +20873,13 @@
         <v>614</v>
       </c>
       <c r="N318" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O318" t="s">
-        <v>816</v>
+        <v>893</v>
+      </c>
+      <c r="P318" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="319" spans="4:23" x14ac:dyDescent="0.25">
@@ -20892,10 +20904,10 @@
         <v>614</v>
       </c>
       <c r="N319" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O319" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="320" spans="4:23" x14ac:dyDescent="0.25">
@@ -20935,10 +20947,10 @@
         <v>614</v>
       </c>
       <c r="N321" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O321" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="322" spans="4:23" x14ac:dyDescent="0.25">
@@ -20998,13 +21010,13 @@
         <v>614</v>
       </c>
       <c r="N325" t="s">
+        <v>825</v>
+      </c>
+      <c r="O325" t="s">
         <v>826</v>
       </c>
-      <c r="O325" t="s">
-        <v>827</v>
-      </c>
       <c r="W325" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="326" spans="4:23" x14ac:dyDescent="0.25">
@@ -21023,16 +21035,16 @@
       <c r="J326" s="3"/>
       <c r="K326" s="41"/>
       <c r="L326" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M326" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N326" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="O326" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="327" spans="4:23" x14ac:dyDescent="0.25">
@@ -21068,16 +21080,16 @@
       </c>
       <c r="K328" s="41"/>
       <c r="L328" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M328" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N328" t="s">
+        <v>825</v>
+      </c>
+      <c r="O328" t="s">
         <v>826</v>
-      </c>
-      <c r="O328" t="s">
-        <v>827</v>
       </c>
       <c r="P328" t="s">
         <v>811</v>
@@ -21104,16 +21116,16 @@
       </c>
       <c r="K329" s="41"/>
       <c r="L329" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M329" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N329" t="s">
+        <v>825</v>
+      </c>
+      <c r="O329" t="s">
         <v>826</v>
-      </c>
-      <c r="O329" t="s">
-        <v>827</v>
       </c>
       <c r="P329" t="s">
         <v>811</v>
@@ -21140,16 +21152,16 @@
       </c>
       <c r="K330" s="41"/>
       <c r="L330" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M330" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N330" t="s">
+        <v>825</v>
+      </c>
+      <c r="O330" t="s">
         <v>826</v>
-      </c>
-      <c r="O330" t="s">
-        <v>827</v>
       </c>
       <c r="P330" t="s">
         <v>811</v>
@@ -21240,16 +21252,16 @@
         <v>614</v>
       </c>
       <c r="N335" t="s">
+        <v>825</v>
+      </c>
+      <c r="O335" t="s">
         <v>826</v>
       </c>
-      <c r="O335" t="s">
-        <v>827</v>
-      </c>
       <c r="P335" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="Q335" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="336" spans="4:23" x14ac:dyDescent="0.25">
@@ -21270,13 +21282,13 @@
       </c>
       <c r="K336" s="41"/>
       <c r="L336" s="52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M336" s="28" t="s">
         <v>614</v>
       </c>
       <c r="N336" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="337" spans="2:23" x14ac:dyDescent="0.25">
@@ -21325,7 +21337,7 @@
       </c>
       <c r="K338" s="41"/>
       <c r="L338" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="M338" s="28"/>
       <c r="W338" s="12" t="s">
@@ -21635,7 +21647,7 @@
       </c>
       <c r="K355" s="42"/>
       <c r="L355" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="M355" s="28"/>
     </row>
@@ -21737,7 +21749,7 @@
       <c r="J360" s="48"/>
       <c r="K360" s="42"/>
       <c r="L360" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="M360" s="28"/>
       <c r="N360"/>
@@ -21768,7 +21780,7 @@
       </c>
       <c r="K361" s="42"/>
       <c r="L361" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="M361" s="28"/>
       <c r="W361" t="s">
@@ -21852,7 +21864,7 @@
       </c>
       <c r="K364" s="42"/>
       <c r="L364" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="M364" s="28"/>
     </row>
@@ -21874,7 +21886,7 @@
       </c>
       <c r="K365" s="42"/>
       <c r="L365" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="M365" s="28"/>
     </row>
@@ -22249,18 +22261,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22283,14 +22295,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A063DF-C20D-4ECC-82E2-4426FC58ED35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB16FA7A-ACFB-4C38-A18E-DC983B68CDC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="0298a7ca-5e45-41ce-82dd-77fd4fe196fc"/>
@@ -22307,6 +22311,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A063DF-C20D-4ECC-82E2-4426FC58ED35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{44ae014c-8170-484b-8a8e-3a6b842e2604}" enabled="1" method="Privileged" siteId="{ad221784-72a8-4263-ac86-0ccc6b152cd8}" removed="0"/>

</xml_diff>